<commit_message>
Update IExcel - Update Excel Export
</commit_message>
<xml_diff>
--- a/ExportExcel/Add Academic Degrees Test.xlsx
+++ b/ExportExcel/Add Academic Degrees Test.xlsx
@@ -12,11 +12,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="26">
+  <si>
+    <t>STT</t>
+  </si>
   <si>
     <t>Test Case Name</t>
   </si>
   <si>
+    <t>Test Name</t>
+  </si>
+  <si>
     <t>Status</t>
   </si>
   <si>
@@ -29,10 +35,13 @@
     <t>testAddADMSucces</t>
   </si>
   <si>
+    <t>TC_AddADM_01</t>
+  </si>
+  <si>
     <t>PASSED</t>
   </si>
   <si>
-    <t>5920 ms</t>
+    <t>6560 ms</t>
   </si>
   <si>
     <t/>
@@ -41,31 +50,46 @@
     <t>testAddADMErrorWithDataMaxLength</t>
   </si>
   <si>
-    <t>7570 ms</t>
+    <t>TC_AddADM_02</t>
+  </si>
+  <si>
+    <t>7558 ms</t>
   </si>
   <si>
     <t>testAddADMErrorWithDataEmpty</t>
   </si>
   <si>
-    <t>8555 ms</t>
+    <t>TC_AddADM_03</t>
+  </si>
+  <si>
+    <t>8436 ms</t>
   </si>
   <si>
     <t>testAddADMErrorWithDuplicateID</t>
   </si>
   <si>
-    <t>5615 ms</t>
+    <t>TC_AddADM_04</t>
+  </si>
+  <si>
+    <t>5612 ms</t>
   </si>
   <si>
     <t>testAddADMErrorWithInvalidFormat</t>
   </si>
   <si>
-    <t>8453 ms</t>
+    <t>TC_AddADM_05</t>
+  </si>
+  <si>
+    <t>8318 ms</t>
   </si>
   <si>
     <t>testAddADMErrorWithDataMinLength</t>
   </si>
   <si>
-    <t>5331 ms</t>
+    <t>TC_AddADM_06</t>
+  </si>
+  <si>
+    <t>5272 ms</t>
   </si>
 </sst>
 </file>
@@ -82,12 +106,32 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="darkGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="42"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="42"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -102,24 +146,28 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
   </cellXfs>
 </styleSheet>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="31.9609375" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="7.08203125" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="13.2109375" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="18.703125" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="3.76171875" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="31.9609375" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="14.16796875" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="7.08203125" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="13.2109375" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="18.703125" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -135,89 +183,131 @@
       <c r="D1" t="s" s="0">
         <v>3</v>
       </c>
+      <c r="E1" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s" s="0">
+        <v>5</v>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" t="s" s="0">
-        <v>4</v>
+      <c r="A2" t="n" s="0">
+        <v>1.0</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>6</v>
-      </c>
-      <c r="D2" t="s" s="0">
         <v>7</v>
       </c>
+      <c r="D2" t="s" s="1">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="F2" t="s" s="0">
+        <v>10</v>
+      </c>
     </row>
     <row r="3">
-      <c r="A3" t="s" s="0">
-        <v>8</v>
+      <c r="A3" t="n" s="0">
+        <v>2.0</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s" s="0">
-        <v>9</v>
-      </c>
-      <c r="D3" t="s" s="0">
-        <v>7</v>
+        <v>12</v>
+      </c>
+      <c r="D3" t="s" s="1">
+        <v>8</v>
+      </c>
+      <c r="E3" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="F3" t="s" s="0">
+        <v>10</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="s" s="0">
-        <v>10</v>
+      <c r="A4" t="n" s="0">
+        <v>3.0</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="C4" t="s" s="0">
-        <v>11</v>
-      </c>
-      <c r="D4" t="s" s="0">
-        <v>7</v>
+        <v>15</v>
+      </c>
+      <c r="D4" t="s" s="1">
+        <v>8</v>
+      </c>
+      <c r="E4" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="F4" t="s" s="0">
+        <v>10</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="s" s="0">
-        <v>12</v>
+      <c r="A5" t="n" s="0">
+        <v>4.0</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="C5" t="s" s="0">
-        <v>13</v>
-      </c>
-      <c r="D5" t="s" s="0">
-        <v>7</v>
+        <v>18</v>
+      </c>
+      <c r="D5" t="s" s="1">
+        <v>8</v>
+      </c>
+      <c r="E5" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="F5" t="s" s="0">
+        <v>10</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="s" s="0">
-        <v>14</v>
+      <c r="A6" t="n" s="0">
+        <v>5.0</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="C6" t="s" s="0">
-        <v>15</v>
-      </c>
-      <c r="D6" t="s" s="0">
-        <v>7</v>
+        <v>21</v>
+      </c>
+      <c r="D6" t="s" s="1">
+        <v>8</v>
+      </c>
+      <c r="E6" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="F6" t="s" s="0">
+        <v>10</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="s" s="0">
-        <v>16</v>
+      <c r="A7" t="n" s="0">
+        <v>6.0</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="C7" t="s" s="0">
-        <v>17</v>
-      </c>
-      <c r="D7" t="s" s="0">
-        <v>7</v>
+        <v>24</v>
+      </c>
+      <c r="D7" t="s" s="1">
+        <v>8</v>
+      </c>
+      <c r="E7" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="F7" t="s" s="0">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Error while verifying user by name: no such element: Unable to locate element
</commit_message>
<xml_diff>
--- a/ExportExcel/Add Academic Degrees Test.xlsx
+++ b/ExportExcel/Add Academic Degrees Test.xlsx
@@ -41,7 +41,7 @@
     <t>PASSED</t>
   </si>
   <si>
-    <t>6008 ms</t>
+    <t>7323 ms</t>
   </si>
   <si>
     <t/>
@@ -53,7 +53,7 @@
     <t>TC_AddADM_02</t>
   </si>
   <si>
-    <t>7710 ms</t>
+    <t>7758 ms</t>
   </si>
   <si>
     <t>testAddADMErrorWithDataEmpty</t>
@@ -62,7 +62,7 @@
     <t>TC_AddADM_03</t>
   </si>
   <si>
-    <t>8533 ms</t>
+    <t>8483 ms</t>
   </si>
   <si>
     <t>testAddADMErrorWithDuplicateID</t>
@@ -71,7 +71,7 @@
     <t>TC_AddADM_04</t>
   </si>
   <si>
-    <t>5694 ms</t>
+    <t>5657 ms</t>
   </si>
   <si>
     <t>testAddADMErrorWithInvalidFormat</t>
@@ -80,7 +80,7 @@
     <t>TC_AddADM_05</t>
   </si>
   <si>
-    <t>8744 ms</t>
+    <t>8345 ms</t>
   </si>
   <si>
     <t>testAddADMErrorWithDataMinLength</t>
@@ -89,7 +89,7 @@
     <t>TC_AddADM_06</t>
   </si>
   <si>
-    <t>6103 ms</t>
+    <t>5336 ms</t>
   </si>
 </sst>
 </file>

</xml_diff>